<commit_message>
Refactor documentation and cleanup scripts: remove demo tasks, update implementation references, and enhance report tracking setup for multi-agent orchestration.
</commit_message>
<xml_diff>
--- a/.docs/report-template.xlsx
+++ b/.docs/report-template.xlsx
@@ -10,8 +10,9 @@
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Tasks" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Waves" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Agents" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Timeline" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Research" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Agents" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Timeline" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -21,7 +22,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -51,8 +52,12 @@
       <b val="1"/>
       <color rgb="00DB2777"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -72,6 +77,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00F9A8D4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005B21B6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009333EA"/>
       </patternFill>
     </fill>
   </fills>
@@ -101,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -114,6 +129,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -572,9 +594,9 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="inlineStr">
-        <is>
-          <t>Total Duration</t>
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>Agent Metrics</t>
         </is>
       </c>
       <c r="B8" s="6" t="inlineStr">
@@ -591,11 +613,11 @@
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>Tokens Used</t>
+          <t>Background CLI Agents</t>
         </is>
       </c>
       <c r="B9" s="4">
-        <f>SUM(Tasks!F:F)</f>
+        <f>COUNTIF(Agents!C:C,"Background CLI")</f>
         <v/>
       </c>
       <c r="C9" s="5" t="inlineStr">
@@ -607,17 +629,28 @@
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>Success Rate</t>
+          <t>Subagent Research Calls</t>
         </is>
       </c>
       <c r="B10" s="6">
-        <f>IF(B5&gt;0,ROUND(B6/B5*100,1)&amp;"%","N/A")</f>
+        <f>COUNTA(Research!A:A)-1</f>
         <v/>
       </c>
       <c r="C10" s="7" t="inlineStr">
         <is>
           <t>Completed/Total</t>
         </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Total Agent Operations</t>
+        </is>
+      </c>
+      <c r="B11">
+        <f>B9+B10</f>
+        <v/>
       </c>
     </row>
     <row r="12">
@@ -691,7 +724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -719,27 +752,32 @@
           <t>Agent</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Duration</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Tokens</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
@@ -815,7 +853,78 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="10" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="12" t="inlineStr">
+        <is>
+          <t>Research ID</t>
+        </is>
+      </c>
+      <c r="B1" s="12" t="inlineStr">
+        <is>
+          <t>After Wave</t>
+        </is>
+      </c>
+      <c r="C1" s="12" t="inlineStr">
+        <is>
+          <t>Purpose</t>
+        </is>
+      </c>
+      <c r="D1" s="12" t="inlineStr">
+        <is>
+          <t>Findings Summary</t>
+        </is>
+      </c>
+      <c r="E1" s="12" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+      <c r="F1" s="12" t="inlineStr">
+        <is>
+          <t>Tokens</t>
+        </is>
+      </c>
+      <c r="G1" s="12" t="inlineStr">
+        <is>
+          <t>Enriched Wave</t>
+        </is>
+      </c>
+      <c r="H1" s="12" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -843,27 +952,32 @@
           <t>Task</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Wave</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Worktree</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Duration</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Tokens</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
@@ -874,7 +988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>